<commit_message>
Update Open Source Tuberculosis Consortium Compounds.xlsx
Upload
</commit_message>
<xml_diff>
--- a/Open Source Tuberculosis Consortium Compounds.xlsx
+++ b/Open Source Tuberculosis Consortium Compounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fahim\Documents\GitHub\OSTB_Series_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43DF461F-1169-4C46-8547-5DB3727BB2A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66196B3A-92E3-4DC4-8CB7-7CB01F8E61E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="522">
   <si>
     <t xml:space="preserve">OSTB ID
 </t>
@@ -1226,9 +1226,6 @@
     <t>JBG27-1-1</t>
   </si>
   <si>
-    <t>JBG29-3-4/ JBG29-4-1/ JBG29-4-2</t>
-  </si>
-  <si>
     <t>OC(C(Cl)=C1)=C(NC(CN2CCOCC2)=O)C(Cl)=C1Cl</t>
   </si>
   <si>
@@ -1406,9 +1403,6 @@
     <t>LKPJKFRGNQQAEI-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>SKF-57841-A</t>
-  </si>
-  <si>
     <t>OC(C(Cl)=C1)=C(NC(CN2CCCC2)=O)C(Cl)=C1Cl</t>
   </si>
   <si>
@@ -1418,9 +1412,6 @@
     <t>WJZKZIGPRKVIBP-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>SKF-57845-A</t>
-  </si>
-  <si>
     <t>OC(C(Cl)=C1)=C(NC(CN2CCCCC2)=O)C(Cl)=C1Cl</t>
   </si>
   <si>
@@ -1430,9 +1421,6 @@
     <t>JSAQWFABXMOLEF-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>SKF-57856-A</t>
-  </si>
-  <si>
     <t>OC(C(Cl)=C1)=C(NC(CN(CC)CC)=O)C(Cl)=C1Cl</t>
   </si>
   <si>
@@ -1442,9 +1430,6 @@
     <t>USDMRGLCXBKDFO-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>SKF-57858-A</t>
-  </si>
-  <si>
     <t>OSTBS99</t>
   </si>
   <si>
@@ -1463,9 +1448,6 @@
     <t>WSBZLMCARLWAEN-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>GSK807337A</t>
-  </si>
-  <si>
     <t>Clc1cc(NC(CN2CCOCC2)=O)c(Cl)cc1</t>
   </si>
   <si>
@@ -1475,9 +1457,6 @@
     <t>ZIWXUBMODWBKQB-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>GSK856324A</t>
-  </si>
-  <si>
     <t>Clc1cc(NC(CN2CCOCC2)=O)cc(Cl)c1</t>
   </si>
   <si>
@@ -1487,9 +1466,6 @@
     <t>NKEOLRWGTITEKX-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>GR200832X</t>
-  </si>
-  <si>
     <t>COc1c(NC(CN2CCOCC2)=O)c(Cl)c(Cl)cc1Cl.Cl</t>
   </si>
   <si>
@@ -1497,9 +1473,6 @@
   </si>
   <si>
     <t>InChI=1S/C13H15Cl3N2O3.ClH/c1-20-13-9(15)6-8(14)11(16)12(13)17-10(19)7-18-2-4-21-5-3-18;/h6H,2-5,7H2,1H3,(H,17,19);1H</t>
-  </si>
-  <si>
-    <t>SKF-57857-A</t>
   </si>
   <si>
     <r>
@@ -1539,12 +1512,108 @@
   <si>
     <t>&lt;</t>
   </si>
+  <si>
+    <t>OSTBL5</t>
+  </si>
+  <si>
+    <t>FI7-1</t>
+  </si>
+  <si>
+    <t>OC(C(Cl)=C1)=C(C(NCCN2CCOCC2)=O)C(Cl)=C1Cl</t>
+  </si>
+  <si>
+    <t>1S/C13H15Cl3N2O3/c14-8-7-9(15)12(19)10(11(8)16)13(20)17-1-2-18-3-5-21-6-4-18/h7,19H,1-6H2,(H,17,20)</t>
+  </si>
+  <si>
+    <t>SBURILLTWGDGHX-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>OSTBL2</t>
+  </si>
+  <si>
+    <t>FI12-2D</t>
+  </si>
+  <si>
+    <t>O=C(CN1CCOCC1)NC2=C([H])C(Cl)=C(O)C(Cl)=C2[H]</t>
+  </si>
+  <si>
+    <t>1S/C12H14Cl2N2O3/c13-9-5-8(6-10(14)12(9)18)15-11(17)7-16-1-3-19-4-2-16/h5-6,18H,1-4,7H2,(H,15,17)</t>
+  </si>
+  <si>
+    <t>ZAIKOSZVKNJROG-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>OSTBL3</t>
+  </si>
+  <si>
+    <t>FI16-1</t>
+  </si>
+  <si>
+    <t>FC1=C(F)C(NC(CN2CCOCC2)=O)=C(F)C(F)=C1</t>
+  </si>
+  <si>
+    <t>1S/C12H12F4N2O2/c13-7-5-8(14)11(16)12(10(7)15)17-9(19)6-18-1-3-20-4-2-18/h5H,1-4,6H2,(H,17,19)</t>
+  </si>
+  <si>
+    <t>SHZLQOYTXDWJDY-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>OSTBL1</t>
+  </si>
+  <si>
+    <t>FI18-1</t>
+  </si>
+  <si>
+    <t>ClC1=CC(NC(CN2CCOCC2)=O)=C(Cl)C(Cl)=C1</t>
+  </si>
+  <si>
+    <t>1S/C12H13Cl3N2O2/c13-8-5-9(14)12(15)10(6-8)16-11(18)7-17-1-3-19-4-2-17/h5-6H,1-4,7H2,(H,16,18)</t>
+  </si>
+  <si>
+    <t>YKJOBONYFFLZPP-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>OSTBL6</t>
+  </si>
+  <si>
+    <t>FI19-1</t>
+  </si>
+  <si>
+    <t>ClC1=C(O)C(S(NCCN2CCOCC2)(=O)=O)=CC(Cl)=C1</t>
+  </si>
+  <si>
+    <t>1S/C12H16Cl2N2O4S/c13-9-7-10(14)12(17)11(8-9)21(18,19)15-1-2-16-3-5-20-6-4-16/h7-8,15,17H,1-6H2</t>
+  </si>
+  <si>
+    <t>ZISORKXNPXVEDY-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>OSTBL4</t>
+  </si>
+  <si>
+    <t>FI22-1</t>
+  </si>
+  <si>
+    <t>ClC1=CC(NC(CN2CCOCC2)=O)=CC(Cl)=N1</t>
+  </si>
+  <si>
+    <t>1S/C11H13Cl2N3O2/c12-9-5-8(6-10(13)15-9)14-11(17)7-16-1-3-18-4-2-16/h5-6H,1-4,7H2,(H,14,15,17)</t>
+  </si>
+  <si>
+    <t>UHWPRBXBKGTUPY-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>FI26-1</t>
+  </si>
+  <si>
+    <t>JBG29-3-4/ JBG29-4-1/ JBG29-4-2/FI10-2 Prep</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1554,20 +1623,24 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1607,6 +1680,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1616,7 +1695,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1624,11 +1703,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1655,9 +1749,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1714,11 +1805,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1726,13 +1835,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1740,6 +1843,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2069,8 +2181,8 @@
   </sheetPr>
   <dimension ref="A1:AK1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2109,34 +2221,34 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>490</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>493</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>494</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>495</v>
+        <v>482</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>484</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>9</v>
@@ -2179,8 +2291,8 @@
       <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>492</v>
+      <c r="H2" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I2" s="3">
         <v>100</v>
@@ -2285,8 +2397,8 @@
       <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>492</v>
+      <c r="H4" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I4" s="3">
         <v>100</v>
@@ -2444,8 +2556,8 @@
       <c r="G7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>492</v>
+      <c r="H7" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I7" s="3">
         <v>100</v>
@@ -2652,8 +2764,8 @@
       <c r="G11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>492</v>
+      <c r="H11" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I11" s="3">
         <v>100</v>
@@ -2705,8 +2817,8 @@
       <c r="G12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>492</v>
+      <c r="H12" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I12" s="3">
         <v>100</v>
@@ -2758,8 +2870,8 @@
       <c r="G13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>492</v>
+      <c r="H13" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I13" s="3">
         <v>100</v>
@@ -2811,8 +2923,8 @@
       <c r="G14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>492</v>
+      <c r="H14" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="I14" s="3">
         <v>100</v>
@@ -2831,9 +2943,9 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="13"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="12"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
@@ -2866,8 +2978,8 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="18" t="s">
-        <v>492</v>
+      <c r="J15" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="K15" s="5">
         <v>125</v>
@@ -3027,8 +3139,8 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="18" t="s">
-        <v>492</v>
+      <c r="J18" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="K18" s="5">
         <v>125</v>
@@ -3188,8 +3300,8 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="18" t="s">
-        <v>492</v>
+      <c r="J21" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="K21" s="5">
         <v>125</v>
@@ -3455,8 +3567,8 @@
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="18" t="s">
-        <v>492</v>
+      <c r="J26" s="17" t="s">
+        <v>483</v>
       </c>
       <c r="K26" s="5">
         <v>125</v>
@@ -6246,14 +6358,14 @@
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-      <c r="L81" s="18"/>
-      <c r="M81" s="18"/>
-      <c r="N81" s="18"/>
-      <c r="O81" s="18"/>
-      <c r="P81" s="18"/>
-      <c r="Q81" s="18"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="17"/>
+      <c r="L81" s="17"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
+      <c r="Q81" s="17"/>
       <c r="R81" s="3" t="s">
         <v>384</v>
       </c>
@@ -6299,14 +6411,14 @@
       </c>
       <c r="H82" s="9"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="18"/>
-      <c r="L82" s="18"/>
-      <c r="M82" s="18"/>
-      <c r="N82" s="18"/>
-      <c r="O82" s="18"/>
-      <c r="P82" s="18"/>
-      <c r="Q82" s="18"/>
+      <c r="J82" s="17"/>
+      <c r="K82" s="17"/>
+      <c r="L82" s="17"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
+      <c r="Q82" s="17"/>
       <c r="R82" s="4"/>
       <c r="S82" s="4"/>
       <c r="T82" s="4"/>
@@ -6350,14 +6462,14 @@
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="18"/>
-      <c r="K83" s="18"/>
-      <c r="L83" s="18"/>
-      <c r="M83" s="18"/>
-      <c r="N83" s="18"/>
-      <c r="O83" s="18"/>
-      <c r="P83" s="18"/>
-      <c r="Q83" s="18"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="17"/>
+      <c r="L83" s="17"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="17"/>
+      <c r="Q83" s="17"/>
       <c r="R83" s="4"/>
       <c r="S83" s="4"/>
       <c r="T83" s="4"/>
@@ -6380,51 +6492,51 @@
       <c r="AK83" s="4"/>
     </row>
     <row r="84" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33">
+        <v>3</v>
+      </c>
+      <c r="E84" s="37" t="s">
         <v>398</v>
       </c>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30">
-        <v>3</v>
-      </c>
-      <c r="E84" s="32" t="s">
+      <c r="F84" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="F84" s="32" t="s">
+      <c r="G84" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="G84" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="H84" s="33"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="30" t="s">
-        <v>492</v>
-      </c>
-      <c r="K84" s="29">
+      <c r="H84" s="34"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="33" t="s">
+        <v>483</v>
+      </c>
+      <c r="K84" s="35">
         <v>125</v>
       </c>
-      <c r="L84" s="29"/>
-      <c r="M84" s="29">
+      <c r="L84" s="35"/>
+      <c r="M84" s="35">
         <v>2.0099999999999998</v>
       </c>
-      <c r="N84" s="27" t="s">
-        <v>496</v>
-      </c>
-      <c r="O84" s="17">
+      <c r="N84" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="O84" s="16">
         <v>0.48</v>
       </c>
-      <c r="P84" s="35" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q84" s="10">
+      <c r="P84" s="41" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q84" s="42">
         <v>4</v>
       </c>
-      <c r="R84" s="36"/>
-      <c r="S84" s="36"/>
+      <c r="R84" s="39"/>
+      <c r="S84" s="39"/>
       <c r="T84" s="5"/>
       <c r="U84" s="5"/>
       <c r="V84" s="5"/>
@@ -6445,29 +6557,29 @@
       <c r="AK84" s="5"/>
     </row>
     <row r="85" spans="1:37" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="32"/>
-      <c r="H85" s="33"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="30"/>
-      <c r="K85" s="29"/>
-      <c r="L85" s="29"/>
-      <c r="M85" s="29"/>
-      <c r="N85" s="27" t="s">
-        <v>497</v>
-      </c>
-      <c r="O85" s="17">
+      <c r="A85" s="33"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="34"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="33"/>
+      <c r="K85" s="35"/>
+      <c r="L85" s="35"/>
+      <c r="M85" s="35"/>
+      <c r="N85" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="O85" s="16">
         <v>0.39700000000000002</v>
       </c>
-      <c r="P85" s="35"/>
-      <c r="Q85" s="10"/>
-      <c r="R85" s="36"/>
-      <c r="S85" s="36"/>
+      <c r="P85" s="41"/>
+      <c r="Q85" s="42"/>
+      <c r="R85" s="39"/>
+      <c r="S85" s="39"/>
       <c r="T85" s="4"/>
       <c r="U85" s="4"/>
       <c r="V85" s="4"/>
@@ -6488,34 +6600,34 @@
       <c r="AK85" s="4"/>
     </row>
     <row r="86" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18" t="s">
+      <c r="A86" s="17" t="s">
         <v>389</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17">
+        <v>3</v>
+      </c>
+      <c r="E86" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18">
-        <v>3</v>
-      </c>
-      <c r="E86" s="20" t="s">
+      <c r="F86" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="F86" s="20" t="s">
+      <c r="G86" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="G86" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="H86" s="15"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="18"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="23"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="12"/>
-      <c r="R86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="17"/>
+      <c r="K86" s="22"/>
+      <c r="L86" s="22"/>
+      <c r="M86" s="22"/>
+      <c r="P86" s="16"/>
+      <c r="Q86" s="11"/>
+      <c r="R86" s="13"/>
       <c r="S86" s="4"/>
       <c r="T86" s="4"/>
       <c r="U86" s="4"/>
@@ -6537,36 +6649,36 @@
       <c r="AK86" s="4"/>
     </row>
     <row r="87" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18">
+      <c r="A87" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17">
         <v>3</v>
       </c>
-      <c r="E87" s="20" t="s">
+      <c r="E87" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="F87" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="F87" s="20" t="s">
+      <c r="G87" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="G87" s="20" t="s">
-        <v>408</v>
-      </c>
-      <c r="H87" s="15"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="18"/>
-      <c r="K87" s="18"/>
-      <c r="L87" s="18"/>
-      <c r="M87" s="18"/>
-      <c r="N87" s="18"/>
-      <c r="O87" s="18"/>
-      <c r="P87" s="18"/>
-      <c r="Q87" s="18"/>
-      <c r="R87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="17"/>
+      <c r="L87" s="17"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
+      <c r="Q87" s="17"/>
+      <c r="R87" s="13"/>
       <c r="S87" s="4"/>
       <c r="T87" s="4"/>
       <c r="U87" s="4"/>
@@ -6588,36 +6700,36 @@
       <c r="AK87" s="4"/>
     </row>
     <row r="88" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18">
+      <c r="A88" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17">
         <v>3</v>
       </c>
-      <c r="E88" s="20" t="s">
+      <c r="E88" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="F88" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="F88" s="20" t="s">
+      <c r="G88" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="G88" s="20" t="s">
-        <v>417</v>
-      </c>
-      <c r="H88" s="15"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="18"/>
-      <c r="M88" s="18"/>
-      <c r="N88" s="18"/>
-      <c r="O88" s="18"/>
-      <c r="P88" s="18"/>
-      <c r="Q88" s="18"/>
-      <c r="R88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="17"/>
+      <c r="L88" s="17"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="17"/>
+      <c r="R88" s="13"/>
       <c r="S88" s="4"/>
       <c r="T88" s="4"/>
       <c r="U88" s="4"/>
@@ -6639,36 +6751,36 @@
       <c r="AK88" s="4"/>
     </row>
     <row r="89" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="B89" s="19" t="s">
+      <c r="A89" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17">
+        <v>3</v>
+      </c>
+      <c r="E89" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18">
-        <v>3</v>
-      </c>
-      <c r="E89" s="20" t="s">
+      <c r="F89" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="F89" s="20" t="s">
+      <c r="G89" s="19" t="s">
         <v>421</v>
       </c>
-      <c r="G89" s="20" t="s">
-        <v>422</v>
-      </c>
-      <c r="H89" s="15"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="18"/>
-      <c r="M89" s="18"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-      <c r="R89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="17"/>
+      <c r="K89" s="17"/>
+      <c r="L89" s="17"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
+      <c r="Q89" s="17"/>
+      <c r="R89" s="13"/>
       <c r="S89" s="4"/>
       <c r="T89" s="4"/>
       <c r="U89" s="4"/>
@@ -6690,45 +6802,45 @@
       <c r="AK89" s="4"/>
     </row>
     <row r="90" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18">
+      <c r="A90" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17">
         <v>3</v>
       </c>
-      <c r="E90" s="20" t="s">
+      <c r="E90" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="F90" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="F90" s="20" t="s">
+      <c r="G90" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="G90" s="20" t="s">
-        <v>425</v>
-      </c>
-      <c r="H90" s="15"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="K90" s="22">
+      <c r="H90" s="14"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="K90" s="21">
         <v>125</v>
       </c>
-      <c r="L90" s="22"/>
-      <c r="M90" s="24">
+      <c r="L90" s="21"/>
+      <c r="M90" s="23">
         <v>27.81</v>
       </c>
-      <c r="N90" s="24"/>
-      <c r="O90" s="24"/>
-      <c r="P90" s="24"/>
-      <c r="Q90" s="11">
+      <c r="N90" s="23"/>
+      <c r="O90" s="23"/>
+      <c r="P90" s="23"/>
+      <c r="Q90" s="10">
         <f xml:space="preserve"> 4</f>
         <v>4</v>
       </c>
-      <c r="R90" s="14"/>
+      <c r="R90" s="13"/>
       <c r="S90" s="4"/>
       <c r="T90" s="4"/>
       <c r="U90" s="4"/>
@@ -6750,48 +6862,48 @@
       <c r="AK90" s="4"/>
     </row>
     <row r="91" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18">
+      <c r="A91" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17">
         <v>3</v>
       </c>
-      <c r="E91" s="20" t="s">
+      <c r="E91" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="F91" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="F91" s="20" t="s">
+      <c r="G91" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="G91" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="H91" s="15"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="K91" s="22">
+      <c r="H91" s="14"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="K91" s="21">
         <v>125</v>
       </c>
-      <c r="L91" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="M91" s="24">
+      <c r="L91" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="M91" s="23">
         <v>100</v>
       </c>
-      <c r="N91" s="24"/>
-      <c r="O91" s="24"/>
-      <c r="P91" s="28" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q91" s="11">
+      <c r="N91" s="23"/>
+      <c r="O91" s="23"/>
+      <c r="P91" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q91" s="10">
         <v>4</v>
       </c>
-      <c r="R91" s="14"/>
+      <c r="R91" s="13"/>
       <c r="S91" s="4"/>
       <c r="T91" s="4"/>
       <c r="U91" s="4"/>
@@ -6813,46 +6925,46 @@
       <c r="AK91" s="4"/>
     </row>
     <row r="92" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
-        <v>431</v>
-      </c>
-      <c r="B92" s="19" t="s">
+      <c r="A92" s="17" t="s">
+        <v>430</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>439</v>
+      </c>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17">
+        <v>3</v>
+      </c>
+      <c r="E92" s="19" t="s">
         <v>440</v>
       </c>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18">
-        <v>3</v>
-      </c>
-      <c r="E92" s="20" t="s">
+      <c r="F92" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="F92" s="20" t="s">
+      <c r="G92" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="G92" s="20" t="s">
-        <v>443</v>
-      </c>
-      <c r="H92" s="15"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="K92" s="22">
+      <c r="H92" s="14"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="K92" s="21">
         <v>125</v>
       </c>
-      <c r="L92" s="22"/>
-      <c r="M92" s="24">
+      <c r="L92" s="21"/>
+      <c r="M92" s="23">
         <v>2.58</v>
       </c>
-      <c r="N92" s="24"/>
-      <c r="O92" s="24"/>
-      <c r="P92" s="28" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q92" s="11">
+      <c r="N92" s="23"/>
+      <c r="O92" s="23"/>
+      <c r="P92" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q92" s="10">
         <v>4</v>
       </c>
-      <c r="R92" s="14"/>
+      <c r="R92" s="13"/>
       <c r="S92" s="4"/>
       <c r="T92" s="4"/>
       <c r="U92" s="4"/>
@@ -6874,38 +6986,38 @@
       <c r="AK92" s="4"/>
     </row>
     <row r="93" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>447</v>
-      </c>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18">
+      <c r="A93" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17">
         <v>3</v>
       </c>
-      <c r="E93" s="20" t="s">
+      <c r="E93" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="F93" s="19" t="s">
         <v>444</v>
       </c>
-      <c r="F93" s="20" t="s">
+      <c r="G93" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="G93" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="H93" s="15"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="18"/>
-      <c r="M93" s="24">
+      <c r="H93" s="14"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="17"/>
+      <c r="K93" s="17"/>
+      <c r="L93" s="17"/>
+      <c r="M93" s="23">
         <v>20.84</v>
       </c>
-      <c r="N93" s="24"/>
-      <c r="O93" s="24"/>
-      <c r="P93" s="24"/>
-      <c r="Q93" s="24"/>
-      <c r="R93" s="14"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
+      <c r="P93" s="23"/>
+      <c r="Q93" s="23"/>
+      <c r="R93" s="13"/>
       <c r="S93" s="4"/>
       <c r="T93" s="4"/>
       <c r="U93" s="4"/>
@@ -6927,53 +7039,53 @@
       <c r="AK93" s="4"/>
     </row>
     <row r="94" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
-        <v>433</v>
-      </c>
-      <c r="B94" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30">
+      <c r="A94" s="33" t="s">
+        <v>432</v>
+      </c>
+      <c r="B94" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33">
         <v>3</v>
       </c>
-      <c r="E94" s="32" t="s">
+      <c r="E94" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="F94" s="37" t="s">
+        <v>444</v>
+      </c>
+      <c r="G94" s="37" t="s">
         <v>448</v>
       </c>
-      <c r="F94" s="32" t="s">
-        <v>445</v>
-      </c>
-      <c r="G94" s="32" t="s">
-        <v>449</v>
-      </c>
-      <c r="H94" s="33"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="30" t="s">
-        <v>492</v>
-      </c>
-      <c r="K94" s="29">
+      <c r="H94" s="34"/>
+      <c r="I94" s="38"/>
+      <c r="J94" s="33" t="s">
+        <v>483</v>
+      </c>
+      <c r="K94" s="35">
         <v>125</v>
       </c>
-      <c r="L94" s="29" t="s">
-        <v>492</v>
-      </c>
-      <c r="M94" s="37">
+      <c r="L94" s="35" t="s">
+        <v>483</v>
+      </c>
+      <c r="M94" s="40">
         <v>100</v>
       </c>
-      <c r="N94" s="11" t="s">
-        <v>496</v>
-      </c>
-      <c r="O94" s="11">
+      <c r="N94" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="O94" s="10">
         <v>1.0751999999999999</v>
       </c>
-      <c r="P94" s="35" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q94" s="10">
+      <c r="P94" s="41" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q94" s="42">
         <v>4</v>
       </c>
-      <c r="R94" s="34"/>
-      <c r="S94" s="36"/>
+      <c r="R94" s="38"/>
+      <c r="S94" s="39"/>
       <c r="T94" s="5"/>
       <c r="U94" s="5"/>
       <c r="V94" s="5"/>
@@ -6994,29 +7106,29 @@
       <c r="AK94" s="5"/>
     </row>
     <row r="95" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="33"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="30"/>
-      <c r="K95" s="29"/>
-      <c r="L95" s="29"/>
-      <c r="M95" s="37"/>
-      <c r="N95" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="O95" s="11">
+      <c r="A95" s="33"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="34"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="33"/>
+      <c r="K95" s="35"/>
+      <c r="L95" s="35"/>
+      <c r="M95" s="40"/>
+      <c r="N95" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="O95" s="10">
         <v>0.43269999999999997</v>
       </c>
-      <c r="P95" s="35"/>
-      <c r="Q95" s="10"/>
-      <c r="R95" s="34"/>
-      <c r="S95" s="36"/>
+      <c r="P95" s="41"/>
+      <c r="Q95" s="42"/>
+      <c r="R95" s="38"/>
+      <c r="S95" s="39"/>
       <c r="T95" s="4"/>
       <c r="U95" s="4"/>
       <c r="V95" s="4"/>
@@ -7037,46 +7149,46 @@
       <c r="AK95" s="4"/>
     </row>
     <row r="96" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
-        <v>434</v>
-      </c>
-      <c r="B96" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18">
+      <c r="A96" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17">
         <v>3</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E96" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="F96" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="F96" s="20" t="s">
+      <c r="G96" s="19" t="s">
         <v>452</v>
       </c>
-      <c r="G96" s="20" t="s">
-        <v>453</v>
-      </c>
-      <c r="H96" s="15"/>
-      <c r="I96" s="14"/>
-      <c r="J96" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="K96" s="22">
+      <c r="H96" s="14"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="K96" s="21">
         <v>125</v>
       </c>
-      <c r="L96" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="M96" s="24">
+      <c r="L96" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="M96" s="23">
         <v>100</v>
       </c>
-      <c r="P96" s="28" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q96" s="11">
+      <c r="P96" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q96" s="10">
         <v>4</v>
       </c>
-      <c r="R96" s="14"/>
+      <c r="R96" s="13"/>
       <c r="S96" s="4"/>
       <c r="T96" s="4"/>
       <c r="U96" s="4"/>
@@ -7098,38 +7210,36 @@
       <c r="AK96" s="4"/>
     </row>
     <row r="97" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="B97" s="18" t="s">
-        <v>458</v>
-      </c>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18">
+      <c r="A97" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17">
         <v>3</v>
       </c>
-      <c r="E97" s="20" t="s">
+      <c r="E97" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="F97" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="F97" s="20" t="s">
+      <c r="G97" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="G97" s="20" t="s">
-        <v>457</v>
-      </c>
-      <c r="H97" s="15"/>
-      <c r="I97" s="14"/>
-      <c r="J97" s="18"/>
-      <c r="K97" s="18"/>
-      <c r="L97" s="18"/>
-      <c r="M97" s="24">
+      <c r="H97" s="14"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="17"/>
+      <c r="K97" s="17"/>
+      <c r="L97" s="17"/>
+      <c r="M97" s="23">
         <v>1.69</v>
       </c>
-      <c r="N97" s="24"/>
-      <c r="O97" s="24"/>
-      <c r="P97" s="24"/>
-      <c r="Q97" s="24"/>
-      <c r="R97" s="14"/>
+      <c r="N97" s="23"/>
+      <c r="O97" s="23"/>
+      <c r="P97" s="23"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="13"/>
       <c r="S97" s="4"/>
       <c r="T97" s="4"/>
       <c r="U97" s="4"/>
@@ -7151,38 +7261,36 @@
       <c r="AK97" s="4"/>
     </row>
     <row r="98" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="18" t="s">
-        <v>436</v>
-      </c>
-      <c r="B98" s="18" t="s">
-        <v>462</v>
-      </c>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18">
+      <c r="A98" s="17" t="s">
+        <v>435</v>
+      </c>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17">
         <v>3</v>
       </c>
-      <c r="E98" s="20" t="s">
+      <c r="E98" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="G98" s="19" t="s">
         <v>459</v>
       </c>
-      <c r="F98" s="20" t="s">
-        <v>460</v>
-      </c>
-      <c r="G98" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="H98" s="15"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="18"/>
-      <c r="K98" s="18"/>
-      <c r="L98" s="18"/>
-      <c r="M98" s="24">
+      <c r="H98" s="14"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="17"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="17"/>
+      <c r="M98" s="23">
         <v>2.65</v>
       </c>
-      <c r="N98" s="24"/>
-      <c r="O98" s="24"/>
-      <c r="P98" s="24"/>
-      <c r="Q98" s="24"/>
-      <c r="R98" s="14"/>
+      <c r="N98" s="23"/>
+      <c r="O98" s="23"/>
+      <c r="P98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="13"/>
       <c r="S98" s="4"/>
       <c r="T98" s="4"/>
       <c r="U98" s="4"/>
@@ -7204,38 +7312,36 @@
       <c r="AK98" s="4"/>
     </row>
     <row r="99" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="18" t="s">
-        <v>437</v>
-      </c>
-      <c r="B99" s="18" t="s">
-        <v>466</v>
-      </c>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18">
+      <c r="A99" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17">
         <v>3</v>
       </c>
-      <c r="E99" s="20" t="s">
-        <v>463</v>
-      </c>
-      <c r="F99" s="20" t="s">
-        <v>464</v>
-      </c>
-      <c r="G99" s="20" t="s">
-        <v>465</v>
-      </c>
-      <c r="H99" s="15"/>
-      <c r="I99" s="14"/>
-      <c r="J99" s="18"/>
-      <c r="K99" s="18"/>
-      <c r="L99" s="18"/>
-      <c r="M99" s="24">
+      <c r="E99" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="H99" s="14"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="17"/>
+      <c r="K99" s="17"/>
+      <c r="L99" s="17"/>
+      <c r="M99" s="23">
         <v>2.67</v>
       </c>
-      <c r="N99" s="24"/>
-      <c r="O99" s="24"/>
-      <c r="P99" s="24"/>
-      <c r="Q99" s="24"/>
-      <c r="R99" s="14"/>
+      <c r="N99" s="23"/>
+      <c r="O99" s="23"/>
+      <c r="P99" s="23"/>
+      <c r="Q99" s="23"/>
+      <c r="R99" s="13"/>
       <c r="S99" s="4"/>
       <c r="T99" s="4"/>
       <c r="U99" s="4"/>
@@ -7257,38 +7363,36 @@
       <c r="AK99" s="4"/>
     </row>
     <row r="100" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="18" t="s">
-        <v>438</v>
-      </c>
-      <c r="B100" s="18" t="s">
-        <v>470</v>
-      </c>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18">
+      <c r="A100" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17">
         <v>3</v>
       </c>
-      <c r="E100" s="20" t="s">
-        <v>467</v>
-      </c>
-      <c r="F100" s="20" t="s">
-        <v>468</v>
-      </c>
-      <c r="G100" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="H100" s="15"/>
-      <c r="I100" s="14"/>
-      <c r="J100" s="18"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="18"/>
-      <c r="M100" s="24">
+      <c r="E100" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="F100" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="G100" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="H100" s="14"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="17"/>
+      <c r="K100" s="17"/>
+      <c r="L100" s="17"/>
+      <c r="M100" s="23">
         <v>3.01</v>
       </c>
-      <c r="N100" s="24"/>
-      <c r="O100" s="24"/>
-      <c r="P100" s="24"/>
-      <c r="Q100" s="24"/>
-      <c r="R100" s="14"/>
+      <c r="N100" s="23"/>
+      <c r="O100" s="23"/>
+      <c r="P100" s="23"/>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="13"/>
       <c r="S100" s="4"/>
       <c r="T100" s="4"/>
       <c r="U100" s="4"/>
@@ -7310,40 +7414,40 @@
       <c r="AK100" s="4"/>
     </row>
     <row r="101" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="18" t="s">
-        <v>439</v>
-      </c>
-      <c r="B101" s="18" t="s">
-        <v>477</v>
-      </c>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18">
+      <c r="A101" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17">
         <v>3</v>
       </c>
-      <c r="E101" s="20" t="s">
-        <v>474</v>
-      </c>
-      <c r="F101" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="G101" s="20" t="s">
-        <v>476</v>
-      </c>
-      <c r="H101" s="15"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="18"/>
-      <c r="K101" s="18"/>
-      <c r="L101" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="M101" s="24">
+      <c r="E101" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="F101" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="H101" s="14"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="17"/>
+      <c r="L101" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="M101" s="23">
         <v>100</v>
       </c>
-      <c r="N101" s="24"/>
-      <c r="O101" s="24"/>
-      <c r="P101" s="24"/>
-      <c r="Q101" s="24"/>
-      <c r="R101" s="14"/>
+      <c r="N101" s="23"/>
+      <c r="O101" s="23"/>
+      <c r="P101" s="23"/>
+      <c r="Q101" s="23"/>
+      <c r="R101" s="13"/>
       <c r="S101" s="4"/>
       <c r="T101" s="4"/>
       <c r="U101" s="4"/>
@@ -7365,40 +7469,38 @@
       <c r="AK101" s="4"/>
     </row>
     <row r="102" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="18" t="s">
-        <v>471</v>
-      </c>
-      <c r="B102" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18">
+      <c r="A102" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17">
         <v>3</v>
       </c>
-      <c r="E102" s="20" t="s">
-        <v>478</v>
-      </c>
-      <c r="F102" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="G102" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="H102" s="15"/>
-      <c r="I102" s="14"/>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="M102" s="24">
+      <c r="E102" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="H102" s="14"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="17"/>
+      <c r="L102" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="M102" s="23">
         <v>100</v>
       </c>
-      <c r="N102" s="24"/>
-      <c r="O102" s="24"/>
-      <c r="P102" s="24"/>
-      <c r="Q102" s="24"/>
-      <c r="R102" s="14"/>
+      <c r="N102" s="23"/>
+      <c r="O102" s="23"/>
+      <c r="P102" s="23"/>
+      <c r="Q102" s="23"/>
+      <c r="R102" s="13"/>
       <c r="S102" s="4"/>
       <c r="T102" s="4"/>
       <c r="U102" s="4"/>
@@ -7420,40 +7522,38 @@
       <c r="AK102" s="4"/>
     </row>
     <row r="103" spans="1:37" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
-        <v>472</v>
-      </c>
-      <c r="B103" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18">
+      <c r="A103" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17">
         <v>3</v>
       </c>
-      <c r="E103" s="20" t="s">
-        <v>482</v>
-      </c>
-      <c r="F103" s="20" t="s">
+      <c r="E103" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="G103" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="H103" s="14"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17" t="s">
         <v>483</v>
       </c>
-      <c r="G103" s="20" t="s">
-        <v>484</v>
-      </c>
-      <c r="H103" s="15"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="18"/>
-      <c r="K103" s="18"/>
-      <c r="L103" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="M103" s="24">
+      <c r="M103" s="23">
         <v>100</v>
       </c>
-      <c r="N103" s="24"/>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24"/>
-      <c r="Q103" s="24"/>
-      <c r="R103" s="14"/>
+      <c r="N103" s="23"/>
+      <c r="O103" s="23"/>
+      <c r="P103" s="23"/>
+      <c r="Q103" s="23"/>
+      <c r="R103" s="13"/>
       <c r="S103" s="4"/>
       <c r="T103" s="4"/>
       <c r="U103" s="4"/>
@@ -7474,41 +7574,39 @@
       <c r="AJ103" s="4"/>
       <c r="AK103" s="4"/>
     </row>
-    <row r="104" spans="1:37" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
-        <v>473</v>
-      </c>
-      <c r="B104" s="18" t="s">
-        <v>489</v>
-      </c>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18">
+    <row r="104" spans="1:37" ht="12.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17">
         <v>3</v>
       </c>
-      <c r="E104" s="21" t="s">
-        <v>486</v>
-      </c>
-      <c r="F104" s="21" t="s">
-        <v>487</v>
-      </c>
-      <c r="G104" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="H104" s="16"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="18"/>
-      <c r="K104" s="18"/>
-      <c r="L104" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="M104" s="24">
+      <c r="E104" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="G104" s="20" t="s">
+        <v>480</v>
+      </c>
+      <c r="H104" s="15"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="17"/>
+      <c r="K104" s="17"/>
+      <c r="L104" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="M104" s="23">
         <v>100</v>
       </c>
-      <c r="N104" s="24"/>
-      <c r="O104" s="24"/>
-      <c r="P104" s="24"/>
-      <c r="Q104" s="24"/>
-      <c r="R104" s="14"/>
+      <c r="N104" s="23"/>
+      <c r="O104" s="23"/>
+      <c r="P104" s="23"/>
+      <c r="Q104" s="23"/>
+      <c r="R104" s="13"/>
       <c r="S104" s="4"/>
       <c r="T104" s="4"/>
       <c r="U104" s="4"/>
@@ -7529,14 +7627,26 @@
       <c r="AJ104" s="4"/>
       <c r="AK104" s="4"/>
     </row>
-    <row r="105" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
+    <row r="105" spans="1:37" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="B105" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="C105" s="30"/>
+      <c r="D105" s="29">
+        <v>3</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>492</v>
+      </c>
+      <c r="F105" s="31" t="s">
+        <v>493</v>
+      </c>
+      <c r="G105" s="32" t="s">
+        <v>494</v>
+      </c>
       <c r="H105" s="5"/>
       <c r="I105" s="4"/>
       <c r="J105" s="5"/>
@@ -7568,14 +7678,26 @@
       <c r="AJ105" s="4"/>
       <c r="AK105" s="4"/>
     </row>
-    <row r="106" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
+    <row r="106" spans="1:37" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="B106" s="29" t="s">
+        <v>496</v>
+      </c>
+      <c r="C106" s="30"/>
+      <c r="D106" s="29">
+        <v>3</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F106" s="31" t="s">
+        <v>498</v>
+      </c>
+      <c r="G106" s="31" t="s">
+        <v>499</v>
+      </c>
       <c r="H106" s="5"/>
       <c r="I106" s="4"/>
       <c r="J106" s="5"/>
@@ -7607,14 +7729,26 @@
       <c r="AJ106" s="4"/>
       <c r="AK106" s="4"/>
     </row>
-    <row r="107" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
+    <row r="107" spans="1:37" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="29" t="s">
+        <v>500</v>
+      </c>
+      <c r="B107" s="29" t="s">
+        <v>501</v>
+      </c>
+      <c r="C107" s="30"/>
+      <c r="D107" s="29">
+        <v>3</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>502</v>
+      </c>
+      <c r="F107" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="G107" s="31" t="s">
+        <v>504</v>
+      </c>
       <c r="H107" s="5"/>
       <c r="I107" s="4"/>
       <c r="J107" s="5"/>
@@ -7646,14 +7780,26 @@
       <c r="AJ107" s="4"/>
       <c r="AK107" s="4"/>
     </row>
-    <row r="108" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
+    <row r="108" spans="1:37" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="29" t="s">
+        <v>505</v>
+      </c>
+      <c r="B108" s="29" t="s">
+        <v>506</v>
+      </c>
+      <c r="C108" s="30"/>
+      <c r="D108" s="29">
+        <v>3</v>
+      </c>
+      <c r="E108" s="31" t="s">
+        <v>507</v>
+      </c>
+      <c r="F108" s="31" t="s">
+        <v>508</v>
+      </c>
+      <c r="G108" s="31" t="s">
+        <v>509</v>
+      </c>
       <c r="H108" s="5"/>
       <c r="I108" s="4"/>
       <c r="J108" s="5"/>
@@ -7685,14 +7831,26 @@
       <c r="AJ108" s="4"/>
       <c r="AK108" s="4"/>
     </row>
-    <row r="109" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
+    <row r="109" spans="1:37" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="B109" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="C109" s="30"/>
+      <c r="D109" s="29">
+        <v>3</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>512</v>
+      </c>
+      <c r="F109" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="G109" s="31" t="s">
+        <v>514</v>
+      </c>
       <c r="H109" s="5"/>
       <c r="I109" s="4"/>
       <c r="J109" s="5"/>
@@ -7724,14 +7882,26 @@
       <c r="AJ109" s="4"/>
       <c r="AK109" s="4"/>
     </row>
-    <row r="110" spans="1:37" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
+    <row r="110" spans="1:37" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="29" t="s">
+        <v>515</v>
+      </c>
+      <c r="B110" s="29" t="s">
+        <v>516</v>
+      </c>
+      <c r="C110" s="30"/>
+      <c r="D110" s="29">
+        <v>3</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="F110" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="G110" s="31" t="s">
+        <v>519</v>
+      </c>
       <c r="H110" s="5"/>
       <c r="I110" s="4"/>
       <c r="J110" s="5"/>
@@ -42514,11 +42684,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="B94:B95"/>
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="L94:L95"/>
     <mergeCell ref="K94:K95"/>
@@ -42526,6 +42691,11 @@
     <mergeCell ref="I94:I95"/>
     <mergeCell ref="H94:H95"/>
     <mergeCell ref="G94:G95"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="B94:B95"/>
     <mergeCell ref="R84:R85"/>
     <mergeCell ref="S84:S85"/>
     <mergeCell ref="M94:M95"/>
@@ -42533,14 +42703,14 @@
     <mergeCell ref="Q94:Q95"/>
     <mergeCell ref="R94:R95"/>
     <mergeCell ref="S94:S95"/>
+    <mergeCell ref="Q84:Q85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="M84:M85"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="D84:D85"/>
     <mergeCell ref="H84:H85"/>
     <mergeCell ref="C84:C85"/>
     <mergeCell ref="L84:L85"/>
-    <mergeCell ref="Q84:Q85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="M84:M85"/>
     <mergeCell ref="J84:J85"/>
     <mergeCell ref="K84:K85"/>
     <mergeCell ref="B84:B85"/>
@@ -42558,5 +42728,6 @@
     <hyperlink ref="R2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>